<commit_message>
Update on Trial Chi Square
</commit_message>
<xml_diff>
--- a/__ output (8-10-2020)/_last/[ ! ] - Chi-Test - b1 (1-Male ; 2-Female) & b5(0-X ; 1-Urban).xlsx
+++ b/__ output (8-10-2020)/_last/[ ! ] - Chi-Test - b1 (1-Male ; 2-Female) & b5(0-X ; 1-Urban).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Candy\Documents\GitHub\OOTO Miner Python v2\__ output (8-10-2020)\_last\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13C1D60-C679-4CDB-B047-0206AF278A78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEDFA03-DF90-4F25-8212-92E2F9264EAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="6204" windowWidth="23040" windowHeight="6876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="1356" windowWidth="23040" windowHeight="6876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1643,13 +1643,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="39.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">

</xml_diff>